<commit_message>
Started to implement forecast performance comparrision
</commit_message>
<xml_diff>
--- a/Model_Parameter.xlsx
+++ b/Model_Parameter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/185c352134c95a0e/Dokumente/Uni_Stoff/Bachelor Thesis/Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian\OneDrive\Dokumente\Uni_Stoff\Bachelor Thesis\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{FA83A6FB-5A43-4FB4-8231-235DDE36D675}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{2BC3BE30-9AE0-4A52-9BF3-CBEB5A370E97}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{FA83A6FB-5A43-4FB4-8231-235DDE36D675}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{48DDFD69-4326-41F8-AFC6-0C86B30AD9D9}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="4365" windowWidth="18000" windowHeight="11055" xr2:uid="{F3800AA9-91BC-44F6-89F7-82C28B46C7D7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F3800AA9-91BC-44F6-89F7-82C28B46C7D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -413,7 +413,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +452,7 @@
         <v>0.21</v>
       </c>
       <c r="F2" s="1">
-        <v>7.6950000000000003</v>
+        <v>7.7214</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -469,7 +469,7 @@
         <v>0.21</v>
       </c>
       <c r="F3" s="1">
-        <v>7.702</v>
+        <v>7.7594000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -486,7 +486,7 @@
         <v>0.21</v>
       </c>
       <c r="F4" s="1">
-        <v>7.7634999999999996</v>
+        <v>7.7618</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -509,7 +509,7 @@
         <v>0.31</v>
       </c>
       <c r="F6" s="1">
-        <v>5.7111000000000001</v>
+        <v>5.9039999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -526,7 +526,7 @@
         <v>0.41</v>
       </c>
       <c r="F7" s="1">
-        <v>5.726</v>
+        <v>5.9157999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -543,7 +543,7 @@
         <v>0.21</v>
       </c>
       <c r="F8" s="1">
-        <v>5.7413999999999996</v>
+        <v>5.9353999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>